<commit_message>
Adding Word document for feedback
</commit_message>
<xml_diff>
--- a/docs/data/datasets.xlsx
+++ b/docs/data/datasets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masonyoungblood/Documents/Work/Spring 2024/Whale ZLA/whale_song_efficiency/docs/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masonyoungblood/Documents/Work/Spring 2024/Whale ZLA/whale_efficiency/docs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09DEE5B-E4DA-964B-AB15-3F4F2523923F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26ACF7-020B-5B40-B800-52A4D0EC0112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{169B7412-2FD3-474B-85B6-D739F0C7EFC2}"/>
+    <workbookView xWindow="63200" yWindow="-6200" windowWidth="34400" windowHeight="28300" xr2:uid="{169B7412-2FD3-474B-85B6-D739F0C7EFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1286,7 +1286,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating with spectrograms and new text based on feedback
</commit_message>
<xml_diff>
--- a/docs/data/datasets.xlsx
+++ b/docs/data/datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masonyoungblood/Documents/Work/Spring 2024/Whale ZLA/whale_efficiency/docs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26ACF7-020B-5B40-B800-52A4D0EC0112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C241449-CF64-8C46-ADD7-C4F76A661AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="63200" yWindow="-6200" windowWidth="34400" windowHeight="28300" xr2:uid="{169B7412-2FD3-474B-85B6-D739F0C7EFC2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="165">
   <si>
     <t>Species</t>
   </si>
@@ -233,9 +233,6 @@
     <t>https://doi.org/10.1073/pnas.2201692119</t>
   </si>
   <si>
-    <t>https://doi.org/10.1002/ece3.9449</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1098/rsos.150372</t>
   </si>
   <si>
@@ -500,9 +497,6 @@
     <t>hersh_etal22</t>
   </si>
   <si>
-    <t>vachon_etal22</t>
-  </si>
-  <si>
     <t>gero_etal16</t>
   </si>
   <si>
@@ -525,6 +519,18 @@
   </si>
   <si>
     <t>Pop sounds are an aggressive display, so not as appropriate for study as the burst pulse signals</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Onset</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1098/rsos.211737</t>
+  </si>
+  <si>
+    <t>vachon_etal22a</t>
   </si>
 </sst>
 </file>
@@ -586,7 +592,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="84">
+    <dxf>
+      <font>
+        <color rgb="FFB600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7C8FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -619,6 +645,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFB600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7C8FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="4" tint="-0.24994659260841701"/>
       </font>
       <fill>
@@ -639,6 +675,76 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7C8FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7C8FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -649,6 +755,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFB600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7C8FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -659,6 +795,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -669,6 +815,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -679,6 +845,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -689,6 +865,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -709,6 +895,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -719,6 +915,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -739,6 +945,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -749,6 +965,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -759,6 +985,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -769,6 +1005,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -779,6 +1025,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -789,6 +1045,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -849,6 +1125,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -859,6 +1155,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -869,6 +1175,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -879,6 +1195,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -919,6 +1255,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -929,6 +1275,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -949,11 +1305,121 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1283,11 +1749,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4686C63-5509-DA4C-BDD2-9CA6DF2804F3}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1299,10 +1765,10 @@
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
     <col min="9" max="9" width="41.6640625" customWidth="1"/>
     <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="11" max="12" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1316,7 +1782,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -1325,22 +1791,25 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1354,28 +1823,27 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" t="s">
         <v>156</v>
       </c>
-      <c r="I2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J2" t="s">
-        <v>158</v>
-      </c>
-      <c r="K2" t="s">
-        <v>123</v>
-      </c>
-      <c r="L2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1389,42 +1857,42 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s">
+        <v>123</v>
+      </c>
+      <c r="K3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>131</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" t="s">
-        <v>124</v>
-      </c>
-      <c r="K3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>132</v>
       </c>
       <c r="F4" t="s">
         <v>53</v>
@@ -1436,7 +1904,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1450,25 +1918,25 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F5" t="s">
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J5" t="s">
-        <v>128</v>
-      </c>
-      <c r="L5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="M5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1482,7 +1950,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F6" t="s">
         <v>53</v>
@@ -1494,7 +1962,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1508,22 +1976,22 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F7" t="s">
         <v>53</v>
       </c>
       <c r="G7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" t="s">
         <v>94</v>
       </c>
-      <c r="I7" t="s">
-        <v>95</v>
-      </c>
-      <c r="L7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1537,28 +2005,31 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F8" t="s">
         <v>53</v>
       </c>
       <c r="G8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" t="s">
         <v>120</v>
       </c>
-      <c r="H8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I8" t="s">
-        <v>121</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1572,7 +2043,7 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -1581,19 +2052,19 @@
         <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1607,7 +2078,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
@@ -1619,7 +2090,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1633,28 +2104,31 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" t="s">
         <v>108</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" t="s">
         <v>109</v>
       </c>
-      <c r="H11" t="s">
-        <v>137</v>
-      </c>
-      <c r="I11" t="s">
-        <v>110</v>
-      </c>
       <c r="J11" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1668,7 +2142,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F12" t="s">
         <v>31</v>
@@ -1677,19 +2151,22 @@
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I12" t="s">
         <v>33</v>
       </c>
       <c r="J12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1703,7 +2180,7 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
         <v>31</v>
@@ -1715,7 +2192,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1729,28 +2206,31 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F14" t="s">
         <v>31</v>
       </c>
       <c r="G14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" t="s">
         <v>67</v>
       </c>
-      <c r="H14" t="s">
-        <v>139</v>
-      </c>
-      <c r="I14" t="s">
-        <v>68</v>
-      </c>
       <c r="J14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1764,28 +2244,31 @@
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F15" t="s">
         <v>31</v>
       </c>
       <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>139</v>
+      </c>
+      <c r="I15" t="s">
         <v>69</v>
       </c>
-      <c r="H15" t="s">
-        <v>140</v>
-      </c>
-      <c r="I15" t="s">
-        <v>70</v>
-      </c>
       <c r="J15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1799,19 +2282,19 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F16" t="s">
         <v>31</v>
       </c>
       <c r="G16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" t="s">
         <v>90</v>
       </c>
-      <c r="I16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1825,19 +2308,19 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" t="s">
         <v>117</v>
       </c>
-      <c r="I17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1851,7 +2334,7 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F18" t="s">
         <v>57</v>
@@ -1863,7 +2346,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1877,63 +2360,69 @@
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" t="s">
         <v>105</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" t="s">
         <v>106</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K19" t="s">
+        <v>122</v>
+      </c>
+      <c r="L19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" t="s">
+        <v>113</v>
+      </c>
+      <c r="G20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
         <v>141</v>
       </c>
-      <c r="I19" t="s">
-        <v>107</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>115</v>
       </c>
-      <c r="H20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I20" t="s">
-        <v>116</v>
-      </c>
       <c r="J20" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1947,31 +2436,31 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K21" t="s">
-        <v>122</v>
-      </c>
-      <c r="L21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="M21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1985,31 +2474,31 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" t="s">
+        <v>142</v>
+      </c>
+      <c r="I22" t="s">
         <v>79</v>
       </c>
-      <c r="H22" t="s">
-        <v>143</v>
-      </c>
-      <c r="I22" t="s">
-        <v>80</v>
-      </c>
       <c r="J22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K22" t="s">
-        <v>122</v>
-      </c>
-      <c r="L22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="M22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -2023,31 +2512,31 @@
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I23" t="s">
         <v>81</v>
       </c>
-      <c r="G23" t="s">
+      <c r="J23" t="s">
+        <v>124</v>
+      </c>
+      <c r="K23" t="s">
+        <v>121</v>
+      </c>
+      <c r="M23" t="s">
         <v>83</v>
       </c>
-      <c r="H23" t="s">
-        <v>145</v>
-      </c>
-      <c r="I23" t="s">
-        <v>82</v>
-      </c>
-      <c r="J23" t="s">
-        <v>125</v>
-      </c>
-      <c r="K23" t="s">
-        <v>122</v>
-      </c>
-      <c r="L23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -2061,28 +2550,28 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
         <v>71</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
+        <v>145</v>
+      </c>
+      <c r="I24" t="s">
         <v>72</v>
       </c>
-      <c r="H24" t="s">
-        <v>146</v>
-      </c>
-      <c r="I24" t="s">
-        <v>73</v>
-      </c>
       <c r="J24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2096,28 +2585,28 @@
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2131,19 +2620,19 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" t="s">
+        <v>98</v>
+      </c>
+      <c r="I26" t="s">
         <v>99</v>
       </c>
-      <c r="I26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -2157,7 +2646,7 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F27" t="s">
         <v>7</v>
@@ -2169,11 +2658,11 @@
         <v>15</v>
       </c>
       <c r="J27" s="2"/>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2187,7 +2676,7 @@
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F28" t="s">
         <v>7</v>
@@ -2200,7 +2689,7 @@
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2214,7 +2703,7 @@
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
@@ -2223,19 +2712,22 @@
         <v>27</v>
       </c>
       <c r="H29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K29" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -2249,7 +2741,7 @@
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F30" t="s">
         <v>7</v>
@@ -2261,7 +2753,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -2275,7 +2767,7 @@
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F31" t="s">
         <v>26</v>
@@ -2284,19 +2776,22 @@
         <v>25</v>
       </c>
       <c r="H31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I31" t="s">
         <v>24</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K31" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2310,7 +2805,7 @@
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F32" t="s">
         <v>48</v>
@@ -2322,7 +2817,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -2336,28 +2831,31 @@
         <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F33" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" t="s">
         <v>111</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
+        <v>148</v>
+      </c>
+      <c r="I33" t="s">
         <v>112</v>
       </c>
-      <c r="H33" t="s">
-        <v>149</v>
-      </c>
-      <c r="I33" t="s">
-        <v>113</v>
-      </c>
       <c r="J33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K33" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -2371,19 +2869,19 @@
         <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F34" t="s">
         <v>49</v>
       </c>
       <c r="G34" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34" t="s">
         <v>88</v>
       </c>
-      <c r="I34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2397,7 +2895,7 @@
         <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F35" t="s">
         <v>49</v>
@@ -2409,7 +2907,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -2423,7 +2921,7 @@
         <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F36" t="s">
         <v>38</v>
@@ -2435,7 +2933,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -2449,7 +2947,7 @@
         <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F37" t="s">
         <v>38</v>
@@ -2461,7 +2959,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -2475,7 +2973,7 @@
         <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
@@ -2484,19 +2982,19 @@
         <v>16</v>
       </c>
       <c r="H38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K38" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2510,28 +3008,31 @@
         <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F39" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" t="s">
         <v>96</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
+        <v>150</v>
+      </c>
+      <c r="I39" t="s">
         <v>97</v>
       </c>
-      <c r="H39" t="s">
-        <v>151</v>
-      </c>
-      <c r="I39" t="s">
-        <v>98</v>
-      </c>
       <c r="J39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K39" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -2545,7 +3046,7 @@
         <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F40" t="s">
         <v>43</v>
@@ -2557,7 +3058,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -2571,28 +3072,28 @@
         <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F41" t="s">
         <v>43</v>
       </c>
       <c r="G41" t="s">
+        <v>91</v>
+      </c>
+      <c r="H41" t="s">
+        <v>151</v>
+      </c>
+      <c r="I41" t="s">
         <v>92</v>
       </c>
-      <c r="H41" t="s">
-        <v>152</v>
-      </c>
-      <c r="I41" t="s">
-        <v>93</v>
-      </c>
       <c r="J41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K41" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2606,7 +3107,7 @@
         <v>11</v>
       </c>
       <c r="E42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F42" t="s">
         <v>60</v>
@@ -2615,19 +3116,22 @@
         <v>61</v>
       </c>
       <c r="H42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I42" t="s">
         <v>64</v>
       </c>
       <c r="J42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K42" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2641,7 +3145,7 @@
         <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F43" t="s">
         <v>60</v>
@@ -2650,19 +3154,22 @@
         <v>62</v>
       </c>
       <c r="H43" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="I43" t="s">
-        <v>65</v>
+        <v>163</v>
       </c>
       <c r="J43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K43" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="L43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2676,7 +3183,7 @@
         <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F44" t="s">
         <v>60</v>
@@ -2685,160 +3192,195 @@
         <v>63</v>
       </c>
       <c r="H44" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K44" t="s">
-        <v>123</v>
+        <v>122</v>
+      </c>
+      <c r="L44" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:L44">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M44">
     <sortCondition ref="F1:F44"/>
   </sortState>
   <conditionalFormatting sqref="E4:E8">
-    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="54" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="55" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="56" operator="equal">
       <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="47" operator="equal">
-      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="34" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="51" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="52" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="53" operator="equal">
       <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="43" operator="equal">
-      <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:E20">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="39" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="40" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="41" operator="equal">
       <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
-      <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:E26">
-    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="30" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="31" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="32" operator="equal">
       <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
-      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:E35">
-    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="24" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="25" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="26" operator="equal">
       <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
-      <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="21" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="22" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="23" operator="equal">
       <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
-      <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E44">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="12" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="14" operator="equal">
       <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
-      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2 A2:D44">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="10" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="11" operator="equal">
       <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
-      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:H9">
-    <cfRule type="cellIs" dxfId="13" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="210" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="211" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="212" operator="equal">
       <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="203" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="202" operator="equal">
-      <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3 H8:H9 H11:H12 H14:H15 H19:H25 H29 H31 H33 F37:H44 J41:J44">
-    <cfRule type="cellIs" dxfId="10" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="114" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="115" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="106" operator="equal">
-      <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="116" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="7" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="108" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="109" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="110" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="101" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K44 L8 L11:L12 L14:L15 L31 L39">
+    <cfRule type="cellIs" dxfId="12" priority="99" stopIfTrue="1" operator="equal">
+      <formula>"Durations"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="100" stopIfTrue="1" operator="equal">
+      <formula>"Intervals"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M6">
+    <cfRule type="cellIs" dxfId="53" priority="231" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="232" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="100" operator="equal">
-      <formula>"?"</formula>
+    <cfRule type="cellIs" dxfId="51" priority="233" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K44">
-    <cfRule type="cellIs" dxfId="4" priority="92" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="L19">
+    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Durations"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Intervals"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="91" stopIfTrue="1" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L20">
+    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Durations"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Intervals"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6">
-    <cfRule type="cellIs" dxfId="2" priority="223" operator="equal">
-      <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="224" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="225" operator="equal">
-      <formula>"Yes"</formula>
+  <conditionalFormatting sqref="L33">
+    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Durations"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Intervals"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L42:L44">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Durations"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Intervals"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Edits based on feedback, preparing for submission
</commit_message>
<xml_diff>
--- a/docs/data/datasets.xlsx
+++ b/docs/data/datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masonyoungblood/Documents/Work/Spring 2024/Whale ZLA/whale_efficiency/docs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C241449-CF64-8C46-ADD7-C4F76A661AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CF73E3-8C15-1C46-B01D-6B1CF5C3B49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="63200" yWindow="-6200" windowWidth="34400" windowHeight="28300" xr2:uid="{169B7412-2FD3-474B-85B6-D739F0C7EFC2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="168">
   <si>
     <t>Species</t>
   </si>
@@ -531,6 +531,15 @@
   </si>
   <si>
     <t>vachon_etal22a</t>
+  </si>
+  <si>
+    <t>Cerchio &amp; Weir (2022)</t>
+  </si>
+  <si>
+    <t>cerchio_weir22</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1098/rsos.220738</t>
   </si>
 </sst>
 </file>
@@ -583,16 +592,77 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFB600FF"/>
@@ -615,6 +685,86 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFB600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7C8FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7C8FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7C8FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -625,6 +775,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -635,6 +805,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -645,81 +825,31 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFB600FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF7C8FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB600FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF7C8FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB600FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF7C8FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB600FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF7C8FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -735,6 +865,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -745,6 +885,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -755,21 +925,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFB600FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF7C8FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -785,6 +955,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -795,6 +975,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -805,6 +1015,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -815,6 +1035,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -825,611 +1065,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1749,11 +1389,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4686C63-5509-DA4C-BDD2-9CA6DF2804F3}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3107,28 +2747,25 @@
         <v>11</v>
       </c>
       <c r="E42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F42" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="G42" t="s">
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="H42" t="s">
-        <v>152</v>
-      </c>
-      <c r="I42" t="s">
-        <v>64</v>
+        <v>166</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="J42" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K42" t="s">
-        <v>122</v>
-      </c>
-      <c r="L42" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -3151,13 +2788,13 @@
         <v>60</v>
       </c>
       <c r="G43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H43" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="I43" t="s">
-        <v>163</v>
+        <v>64</v>
       </c>
       <c r="J43" t="s">
         <v>128</v>
@@ -3189,13 +2826,13 @@
         <v>60</v>
       </c>
       <c r="G44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H44" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="I44" t="s">
-        <v>65</v>
+        <v>163</v>
       </c>
       <c r="J44" t="s">
         <v>128</v>
@@ -3207,187 +2844,228 @@
         <v>12</v>
       </c>
     </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>131</v>
+      </c>
+      <c r="F45" t="s">
+        <v>60</v>
+      </c>
+      <c r="G45" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45" t="s">
+        <v>153</v>
+      </c>
+      <c r="I45" t="s">
+        <v>65</v>
+      </c>
+      <c r="J45" t="s">
+        <v>128</v>
+      </c>
+      <c r="K45" t="s">
+        <v>122</v>
+      </c>
+      <c r="L45" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M44">
-    <sortCondition ref="F1:F44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M45">
+    <sortCondition ref="F1:F45"/>
   </sortState>
   <conditionalFormatting sqref="E4:E8">
-    <cfRule type="cellIs" dxfId="83" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="57" operator="equal">
       <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="55" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="56" operator="equal">
-      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="80" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="56" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="55" operator="equal">
       <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="53" operator="equal">
-      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:E20">
-    <cfRule type="cellIs" dxfId="77" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="44" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
       <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="41" operator="equal">
-      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:E26">
-    <cfRule type="cellIs" dxfId="74" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="31" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="32" operator="equal">
-      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:E35">
-    <cfRule type="cellIs" dxfId="71" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="28" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="27" operator="equal">
       <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="25" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="26" operator="equal">
-      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="68" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E44">
-    <cfRule type="cellIs" dxfId="65" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="15" operator="equal">
       <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="14" operator="equal">
-      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2 A2:D44">
-    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
       <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="10" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="11" operator="equal">
-      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:H9">
-    <cfRule type="cellIs" dxfId="59" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="214" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="213" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="215" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3 H8:H9 H11:H12 H14:H15 H19:H25 H29 H31 H33 F37:H45 J41:J45">
+    <cfRule type="cellIs" dxfId="19" priority="118" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="212" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3 H8:H9 H11:H12 H14:H15 H19:H25 H29 H31 H33 F37:H44 J41:J44">
-    <cfRule type="cellIs" dxfId="4" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="117" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="115" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="119" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="56" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="113" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="112" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="111" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="109" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="110" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K44 L8 L11:L12 L14:L15 L31 L39">
-    <cfRule type="cellIs" dxfId="12" priority="99" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="L8 L11:L12 L14:L15 L31 L39 K2:K45">
+    <cfRule type="cellIs" dxfId="13" priority="102" stopIfTrue="1" operator="equal">
       <formula>"Durations"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="100" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="103" stopIfTrue="1" operator="equal">
+      <formula>"Intervals"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:L20">
+    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Intervals"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Durations"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L33">
+    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Durations"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Intervals"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L42:L44">
+    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Durations"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Intervals"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="cellIs" dxfId="53" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="234" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="235" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="236" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19">
-    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Durations"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"Intervals"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Durations"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Intervals"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L33">
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Durations"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"Intervals"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L42:L44">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"Durations"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Intervals"</formula>
+  <conditionalFormatting sqref="A45:D45">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:D44" xr:uid="{662C56AD-0D04-414F-8E1E-EC75F7C364C9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:D45" xr:uid="{662C56AD-0D04-414F-8E1E-EC75F7C364C9}">
       <formula1>"Yes,?,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K44" xr:uid="{D37E165E-50E5-CC4C-888E-3982989C6CB5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K45" xr:uid="{D37E165E-50E5-CC4C-888E-3982989C6CB5}">
       <formula1>"Durations,Intervals"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>